<commit_message>
completed all the patterns and updated excel sheet with notes
</commit_message>
<xml_diff>
--- a/solved questions.xlsx
+++ b/solved questions.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\problem-solving\interview-prep-coding-questions\coding patterns\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\problem-solving\interview-prep-coding-questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7C067B-D581-47BF-96E6-13DE94E78398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0360CC8B-ED1A-4A88-88D5-417FA60D36FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems divided by pattern" sheetId="1" r:id="rId1"/>
+    <sheet name="Key points" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
   <si>
     <t>Problem Statement</t>
   </si>
@@ -128,13 +129,190 @@
   </si>
   <si>
     <t>Find the duplicate number</t>
+  </si>
+  <si>
+    <t>First missing positive number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclic sort. This had some precomputation as well like extracting only the positive numbers. Also, in this you had to apply some brains on how to leverage cyclic sort as it was not straight forward. </t>
+  </si>
+  <si>
+    <t>Reverse sublist of a linked list</t>
+  </si>
+  <si>
+    <t>In place linked list reversal. In this we just have to think on how to put the pointers in the correct position after we have done the inplace reversal of the LL.</t>
+  </si>
+  <si>
+    <t>In-place reversal of LL</t>
+  </si>
+  <si>
+    <t>Reverse nodes in k group</t>
+  </si>
+  <si>
+    <t>In place linked list reversal. Exactly the same as the previous one, we just need to do it k times.</t>
+  </si>
+  <si>
+    <t>Binary tree level order traversal</t>
+  </si>
+  <si>
+    <t>BFS, nothing much</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>Binary tree zig zag level order traversal</t>
+  </si>
+  <si>
+    <t>BFS, with a flag variable to keep track of when to reverse the intermediate list</t>
+  </si>
+  <si>
+    <t>Sum to root leaf numbers</t>
+  </si>
+  <si>
+    <t>DFS, with just a bit of manipulation. Used recursive as iterative seemed difficult, can explore that part.</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>All paths for a sum</t>
+  </si>
+  <si>
+    <t>Two Heaps</t>
+  </si>
+  <si>
+    <t>Find median from a stream of numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two heaps technique. But you need to remember the algorithm for saving the data and rebalancing when necessary. The algo ensures that one heap always has at max 1 more element than the other heap and whenever this number changes, a rebalancing is done and elements are initially added  only to one heap and rebalanced if necessary. 
+Algo :
+1. Initially add the first element in the max heap
+2. If any number is less than or equal to the maximum element in the max heap then add the number into the max heap else add it to the min heap
+3. After every insert check if the max heap size is greater than the min heap size +1 , if yes then rebalance, that is shift elements from max to min heap
+4. Also check if the min heap size is greater than the max heap, if yes then rebalance.
+</t>
+  </si>
+  <si>
+    <t>Find right interval</t>
+  </si>
+  <si>
+    <t>Two heaps. Extremely difficult, not at all intuitive. Needs practice a hell lot.</t>
+  </si>
+  <si>
+    <t>Subsets</t>
+  </si>
+  <si>
+    <t>Subsets pattern</t>
+  </si>
+  <si>
+    <t>The subsets pattern of finding all the subsets and its awesome !</t>
+  </si>
+  <si>
+    <t>Subsets with duplicates</t>
+  </si>
+  <si>
+    <t>The subsets pattern. Had a bit of play with Java and that's it</t>
+  </si>
+  <si>
+    <t>Letter case permutation</t>
+  </si>
+  <si>
+    <t>The subsets pattern but its much easier with the recursive version of subsets finding and I have used that only</t>
+  </si>
+  <si>
+    <t>Order agnostic binary search</t>
+  </si>
+  <si>
+    <t>The only addition here is that the sort order of the array is not known. This can easily be known by checking if
+arr[start]&lt;=arr[end], in that case the array is surely sorted inascending order , otherwise it is sorted in descending order.</t>
+  </si>
+  <si>
+    <t>Modified Binary Search</t>
+  </si>
+  <si>
+    <t>Find an element in a sorted list of infinite 
+numbers</t>
+  </si>
+  <si>
+    <t>In this the idea is to have the low at 0 and high at 1, if arr[high]&lt;key, that means the key is to the right so we make 
+low as high and high as 2*high, this way we find the bounds first</t>
+  </si>
+  <si>
+    <t>Single element in a sorted array</t>
+  </si>
+  <si>
+    <t>Pretty easy, just a modified version of Binary Search. What you will get confused is when you check for mid-1 and mid+1 and you would want to put boundary checks to avoid IndexOutOfBoundsException but fortunately that won't come up as you are already doing boundary checks. remember if you are not doing boundary checks
+then this solution will fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top k frequent elements </t>
+  </si>
+  <si>
+    <t>Top k elements</t>
+  </si>
+  <si>
+    <t>This uses heap, had difficulties with the java syntax but that's it.</t>
+  </si>
+  <si>
+    <t>K way merge</t>
+  </si>
+  <si>
+    <t>Merge K sorted lists</t>
+  </si>
+  <si>
+    <t>This uses heap, the logic is pretty simple, but since it deals with LL, the shifting of pointers is a nasty affair so be wary of that</t>
+  </si>
+  <si>
+    <t>List is faster than pairs</t>
+  </si>
+  <si>
+    <t>Unordered map is faster than normal map</t>
+  </si>
+  <si>
+    <t>Find K pairs with smallest sums</t>
+  </si>
+  <si>
+    <t>This uses heap, the logic is simple brute force but the only twerk is looking at the pattern of data, i.e, we sort the elements in the priority queue in descding order of sum, so now whenever we encounter two elements whose sum is larger than the largest pair of elements in the heap, then we can break because all the upcoming numbers will have greater sum. This way we are extracting only the smallest k elements.</t>
+  </si>
+  <si>
+    <t>Source: https://hackernoon.com/14-patterns-to-ace-any-coding-interview-question-c5bb3357f6ed</t>
+  </si>
+  <si>
+    <t>Topological sort</t>
+  </si>
+  <si>
+    <t>Implementation of topological sort</t>
+  </si>
+  <si>
+    <t>There are two ways to implement it:
+1. Use DFS, we first go to the deepest point in a path and then keep on adding the nodes into the path as we recurse back
+2. Using the concept of indegrees and queue, where first we add all the nodes into the queue where indegree is zero and then we keep on popping from the queue and reducing the indegree of its adjacent nodes by 1, if the indegree of any adjacent node becomes 0 after reduction then it is added into the queue. And this process is continued until the queue is empty.</t>
+  </si>
+  <si>
+    <t>Task scheduler</t>
+  </si>
+  <si>
+    <t>This uses heap but you need to develop some logic on how to deal with the heap so that the scheduling is done properly</t>
+  </si>
+  <si>
+    <t>Course schedule II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pure topological sort, just one thing, there might be a possibility that there is no valid topological sorting order, in that case we need to return an empty list. So, a bit of logic to check that if all the indegrees in the map is not 0 when the queue is empty, then that means a valid order is not possible </t>
+  </si>
+  <si>
+    <t>Minimum height tree</t>
+  </si>
+  <si>
+    <t>Pure topological sort, but understanding how to use topological sort is extremely difficult here. This is a pretty tough problem, it is rated as medium in Leetcode probably because the code is nothing other than simple topological sort but coming up with the idea on how to use topological sort is extremely difficult.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,8 +328,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,8 +349,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -173,17 +406,175 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -466,188 +857,542 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" customWidth="1"/>
-    <col min="2" max="2" width="36.453125" customWidth="1"/>
-    <col min="3" max="3" width="93.81640625" customWidth="1"/>
+    <col min="1" max="1" width="22.6328125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="36.453125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="93.81640625" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="2" t="s">
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" s="16" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="17" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="8"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+    </row>
+    <row r="27" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+    </row>
+    <row r="29" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="8"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+    </row>
+    <row r="31" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="8"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="8"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+    </row>
+    <row r="33" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="8"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+    </row>
+    <row r="34" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="8"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+    </row>
+    <row r="35" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="8"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="8"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+    </row>
+    <row r="37" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="8"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+    </row>
+    <row r="38" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="22"/>
+      <c r="B40" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="22"/>
+      <c r="B41" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="33"/>
+      <c r="B43" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="32"/>
+      <c r="B44" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="32"/>
+      <c r="B46" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="32"/>
+      <c r="B48" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="33"/>
+      <c r="B50" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="32"/>
+      <c r="B51" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A12"/>
+  <mergeCells count="17">
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C24:C37"/>
+    <mergeCell ref="B24:B37"/>
+    <mergeCell ref="A24:A38"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{CFC1AA7F-202C-49DD-8477-0D68E15CB134}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{69CC30BC-2781-47B2-AD7A-F6A2073B0B75}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{812378D7-0EB7-4E3F-AC00-4AE164987C7B}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{EF6BB714-7155-4145-97CC-EDAF7EFA93E3}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{E3F339C4-9F9E-403F-ACE7-849D7727AAA0}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{47BCDEBE-8816-49DD-BF27-2499AB26A5F6}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{4B2F9616-0A9F-4F13-80AF-AD23B0BFB11B}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{C4FCAD7C-6FE8-42FA-8D96-E699591A49F5}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{D329DDEC-340B-4E80-AD1B-C5F2A32BC923}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{144BC987-115F-4D9E-A336-9E21D007E2EE}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{4DD133C6-0676-43DB-B04F-D74CD113DC29}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{B3009B7B-4455-4CB1-BE83-A32AAB439E51}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{33F565F4-C17F-469E-8FDA-9759D7B21B09}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{A48D9E2B-DF75-469F-9EE7-E87432600AA4}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CFC1AA7F-202C-49DD-8477-0D68E15CB134}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{69CC30BC-2781-47B2-AD7A-F6A2073B0B75}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{812378D7-0EB7-4E3F-AC00-4AE164987C7B}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{EF6BB714-7155-4145-97CC-EDAF7EFA93E3}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{E3F339C4-9F9E-403F-ACE7-849D7727AAA0}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{47BCDEBE-8816-49DD-BF27-2499AB26A5F6}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{4B2F9616-0A9F-4F13-80AF-AD23B0BFB11B}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{C4FCAD7C-6FE8-42FA-8D96-E699591A49F5}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{D329DDEC-340B-4E80-AD1B-C5F2A32BC923}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{144BC987-115F-4D9E-A336-9E21D007E2EE}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{4DD133C6-0676-43DB-B04F-D74CD113DC29}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{B3009B7B-4455-4CB1-BE83-A32AAB439E51}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{33F565F4-C17F-469E-8FDA-9759D7B21B09}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{A48D9E2B-DF75-469F-9EE7-E87432600AA4}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{D30E1573-23EC-4DDF-9C97-5EA101FFAE20}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{2613F280-205E-4A69-9B99-DD5812C1A6D7}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{24A5B3A3-312B-4E8E-8460-AD7D5C3210BE}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{C6B1E268-7990-49E9-9B39-D40C5C540B79}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{BBEE650C-0A59-47BB-AB2D-3A0FC3A4BFBD}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{AB6C9AF3-412F-46BF-9906-B6C66155CDE1}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{7B0C6195-6EA2-49F4-963C-3E3CAB0DBA21}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{FBB52E51-89A0-4295-95E3-EBD09B2B0E59}"/>
+    <hyperlink ref="B38" r:id="rId23" xr:uid="{D590B824-7393-43AF-8882-C2C332213B59}"/>
+    <hyperlink ref="B39" r:id="rId24" xr:uid="{35C5649E-D37C-49F1-BE1A-FE934A20D37E}"/>
+    <hyperlink ref="B40" r:id="rId25" xr:uid="{1B12EF61-C913-47C8-83A4-D5ED80CB9376}"/>
+    <hyperlink ref="B41" r:id="rId26" xr:uid="{B596397C-4EF8-458D-9E7C-05FAC1673763}"/>
+    <hyperlink ref="B42" r:id="rId27" xr:uid="{3D4FDE30-6A80-42FB-ABE8-709F94E3A38C}"/>
+    <hyperlink ref="B43" r:id="rId28" display="https://www.geeksforgeeks.org/find-position-element-sorted-array-infinite-numbers/" xr:uid="{529D1179-D114-4654-91EF-718A204AD6F9}"/>
+    <hyperlink ref="B44" r:id="rId29" xr:uid="{F401B2BB-08CF-4C8C-A9C6-BA790D910C31}"/>
+    <hyperlink ref="B46" r:id="rId30" xr:uid="{88BE921C-A52B-444B-A5AE-BF45F070C1AD}"/>
+    <hyperlink ref="B47" r:id="rId31" xr:uid="{E27FE8F0-A6A9-4EBE-B482-1046087F807F}"/>
+    <hyperlink ref="B48" r:id="rId32" xr:uid="{7F24797A-2C1D-47AB-89B1-7D0E9B28EA2F}"/>
+    <hyperlink ref="B49" r:id="rId33" xr:uid="{D8F3EF91-D92C-4B2E-BD77-F8A8552D28E1}"/>
+    <hyperlink ref="B45" r:id="rId34" xr:uid="{6755566B-4F55-4530-A181-B5A6FA534D39}"/>
+    <hyperlink ref="B50" r:id="rId35" xr:uid="{DF86B085-3BE3-43F8-A721-F4F2845E3F1B}"/>
+    <hyperlink ref="B51" r:id="rId36" xr:uid="{554EA032-DBB8-4B33-AD07-7B304D857D33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446C6DD3-D0DA-421A-A1C2-0B773979D151}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="70.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revised 10 more questions
</commit_message>
<xml_diff>
--- a/solved questions.xlsx
+++ b/solved questions.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\problem-solving\interview-prep-coding-questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0360CC8B-ED1A-4A88-88D5-417FA60D36FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53968479-5548-4E29-BBDE-3C36069244BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems divided by pattern" sheetId="1" r:id="rId1"/>
     <sheet name="Key points" sheetId="3" r:id="rId2"/>
+    <sheet name="Revision" sheetId="4" r:id="rId3"/>
+    <sheet name="Calendar" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="144">
   <si>
     <t>Problem Statement</t>
   </si>
@@ -307,12 +310,217 @@
   <si>
     <t>Pure topological sort, but understanding how to use topological sort is extremely difficult here. This is a pretty tough problem, it is rated as medium in Leetcode probably because the code is nothing other than simple topological sort but coming up with the idea on how to use topological sort is extremely difficult.</t>
   </si>
+  <si>
+    <t>Sometimes to form a relation look at the answers to various inputs</t>
+  </si>
+  <si>
+    <t>The idea to use hashing for a sum check is to save the numbers in one list in a map and then from the other list, pick up a number and check if X-(that number from the other list) is present in the map or not</t>
+  </si>
+  <si>
+    <t>Whenever there is a problem that asks you to tell a number given another relation
+Try out with different inputs and see a pattern, it might use Catalan numbers, Fibonacci numbers etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add two numbers represented as Linked List </t>
+  </si>
+  <si>
+    <t>Problem statement</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Used stacks to represent the two linked lists, then kept on popping, adding and creating the final string, finally converted the string to LL</t>
+  </si>
+  <si>
+    <t>Sort a linked list</t>
+  </si>
+  <si>
+    <t>Simple merge sort technique, the only point is that to find the middle of the linked list we need to use slow and fast pointers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intersection point in a Y shaped LL </t>
+  </si>
+  <si>
+    <t>Two techniques, first is where you find the longer list and then move forward by the difference in the longer list. The second is the hashmap technique but that is not O(1) space</t>
+  </si>
+  <si>
+    <t>Balanced parenthesis</t>
+  </si>
+  <si>
+    <t>Using stacks, this is pretty easy</t>
+  </si>
+  <si>
+    <t>Flattening a LL</t>
+  </si>
+  <si>
+    <t>This is exactly the same problem as merging k sorted LL, you need to use a heap and an array to keep track of the LLs and whose elements you are putting into the heap</t>
+  </si>
+  <si>
+    <t>The celebrity problem</t>
+  </si>
+  <si>
+    <t>This is a very interesting puzzle. The hint is that :
+1. If X knows Y -&gt; X is definitely not a celebrity
+2. If X doesn't know Y -&gt; Y is definitely not a celebrity
+With this idea as the base, we need to keep in mind that at every iteration we can reduce our search space by 1</t>
+  </si>
+  <si>
+    <t>Stock span problem</t>
+  </si>
+  <si>
+    <t>This uses the idea of stack and is similar to the problem "nearest greater element to the left", the idea lies behind how to keep track and leverages the 
+index of the elements in the given array</t>
+  </si>
+  <si>
+    <t>Done using recursion in two ways explained in the "Problems divided by pattern" sheet</t>
+  </si>
+  <si>
+    <t>Generating permutations</t>
+  </si>
+  <si>
+    <t>Very difficult recursion logic, needs several practice to keep it by heart.</t>
+  </si>
+  <si>
+    <t>Next greater element</t>
+  </si>
+  <si>
+    <t>This is done using stacks and is the foundation for Stock span problem , has the same logic</t>
+  </si>
+  <si>
+    <t>Gas Station(Leetcode) / Circular tour(GFG)</t>
+  </si>
+  <si>
+    <t>This is a true brain puzzle and nothing else and can be solved by looking at few properties in the question and the solution is extremely well explained here: 
+https://leetcode.com/problems/gas-station/discuss/1685774/Share-and-explain-my-solution-O(n)-Time-O(1)-Space-no-greedy-no-two-pointer 
+The idea is essentially to find the first index i where gas[i]-cost[i] is not &lt; 0 .
+Now that is our starting position.
+Then from that position we continue till the last position ( the end index) in the array.
+Then we check that the remaining gas that we have after reaching the last position is greater than or equal to the last negative gas-cost.
+If it is then that implies that with that amount of gas, I can easily travel from 0th index to that last negative valued index.
+Hence we are able to determine a circular tour.
+This is a greedy solution, because we are picking up the first value that is non negative and continuing with that</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Task status</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>First non repeating character in a data stream</t>
+  </si>
+  <si>
+    <t>Looks pretty simple with a map and a queue , but I tried with a list and that looks better to me but unfortunately gets a TLE at the 100th test case, need to dig deeper</t>
+  </si>
+  <si>
+    <t>Equilibrium point</t>
+  </si>
+  <si>
+    <t>Pretty simple, uses the prefix sum concept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub array with 0 sum </t>
+  </si>
+  <si>
+    <t>The logic lies in using hashing. So there shall be a sub array with 0 sum only if either or both these cases hold:
+1. There is a prefix sum of value 0
+2. There are two prefix sums with the same value. This is valid because say if at position i , the prefix sum is P and at prefix k the prefix sum is P as well. In that case, this implies that sum of all values from i+1 to k is 0 because sum(0,i) = P and sum(0,k)=P =&gt; sum(0,k)-sum(0,i) =0
+=&gt;{ arr[0]+arr[1]+arr[2]+......arr[i]+arr[i+1]+ ... arr[k] } - { arr[0]+arr[1]+arr[2]+......arr[i] } = 0
+=&gt;   arr[i+1]+ ... arr[k] = 0</t>
+  </si>
+  <si>
+    <t>Longest span in two binary arrays</t>
+  </si>
+  <si>
+    <t>This is a pretty interesting problem and in problems of these types, try to generalise
+ex: 
+Arr 1:  x1 x2 x3 x4 x5
+Arr2:   y1 y2 y3 y4 y5
+Prefix sum of Arr 1:    px1 px2 px3 px4 px5
+Prefix sum of Arr 2:    py1 py2 py3 py4 py5
+Thus, if   pxj - pxi = pyj - pyi ( the sum of numbers from i to j in arr 1 = the sum of numbers from i to j in arr 2)
+Then pxj - pyj = pxi - pyj
+Which implies that if the difference of prefix sum at two points is the same, then the sum is same at that span</t>
+  </si>
+  <si>
+    <t>To check if the sub arrays from i to j in two arrays have the same sum or not, check the two points where the prefix difference is same for both the arrays</t>
+  </si>
+  <si>
+    <t>To check if there is a sub array with 0 sum, then check if there are two values in the prefix sum array having the same sum, or if the prefix sum itself is 0</t>
+  </si>
+  <si>
+    <t>Subarray with given sum</t>
+  </si>
+  <si>
+    <t>This is a pretty simple problem but the solution has quite a number of edge cases which can make your head hurt. It simply uses sliding window but be wary of the edge cases</t>
+  </si>
+  <si>
+    <t>Kadane's algorithm</t>
+  </si>
+  <si>
+    <t>Flip bits</t>
+  </si>
+  <si>
+    <t>The problem looks extremely difficult but when observed properly boils down to a simple problem that can be solved using Kadane's algorithm.
+An awesome explanation provided in this video: https://www.youtube.com/watch?v=Etkf8sRQdbU</t>
+  </si>
+  <si>
+    <t>Game of XOR</t>
+  </si>
+  <si>
+    <t>Simply pattern finding by looking at various inputs. It has been observed that when there are even number of elements, then in all the subarrays combined, each element appears in even numbers, thereby XOR of all elements in all possible sub arrays will eventually reseult to 0
+Similarly it has been observed that when the elements are odd, then except for the odd indexed(0 based indexing) elements, all appears odd number of times, hence XORing only the even indexed elements will result into the solution</t>
+  </si>
+  <si>
+    <t>Swap all odd and even bits</t>
+  </si>
+  <si>
+    <t>This is again a puzzle that requires a bit of your brain in bit magic
+Steps:
+1. Extract all the even bits by doing an AND operation with 0xAAAAAAAA
+2. Extract all the odd bits by doing an AND operation with 0x55555555
+3. Right shift the even bits by 1
+4. Left shift the odd bits by 1
+5. perform OR on the shifted left and right bits</t>
+  </si>
+  <si>
+    <t>A very simple algorithm to find the largest sum contiguous sub array
+The idea to Kadane's algorithm is just that we keep track of the sum of sub array, if by any chance the current sum becomes less than 0, then we start a fresh and make the current sum to 0 so that we can keep track of the sum from the next index</t>
+  </si>
+  <si>
+    <t>Exceptionally odd</t>
+  </si>
+  <si>
+    <t>Simple XOR operation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,8 +543,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +608,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,72 +750,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,6 +821,72 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -859,24 +1170,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="36.453125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="93.81640625" style="25" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="25"/>
+    <col min="1" max="1" width="22.6328125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="36.453125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="93.81640625" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -889,420 +1200,420 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="43"/>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="43"/>
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="44"/>
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="44"/>
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="47"/>
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="47"/>
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="48"/>
+      <c r="B13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15" t="s">
+    <row r="15" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="49"/>
+      <c r="B15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15" t="s">
+    <row r="16" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="49"/>
+      <c r="B16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15" t="s">
+    <row r="17" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="49"/>
+      <c r="B17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18" t="s">
+    <row r="19" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="42"/>
+      <c r="B19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="43"/>
+      <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="44"/>
+      <c r="B23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:3" s="7" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-    </row>
-    <row r="26" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-    </row>
-    <row r="27" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-    </row>
-    <row r="28" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-    </row>
-    <row r="29" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-    </row>
-    <row r="30" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-    </row>
-    <row r="31" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-    </row>
-    <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-    </row>
-    <row r="33" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-    </row>
-    <row r="34" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="8"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-    </row>
-    <row r="35" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="8"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-    </row>
-    <row r="36" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="8"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-    </row>
-    <row r="37" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-    </row>
-    <row r="38" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9" t="s">
+    <row r="25" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="47"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="45"/>
+    </row>
+    <row r="26" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="47"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="45"/>
+    </row>
+    <row r="27" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="47"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="45"/>
+    </row>
+    <row r="28" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="47"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="45"/>
+    </row>
+    <row r="29" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="45"/>
+    </row>
+    <row r="30" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="47"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="45"/>
+    </row>
+    <row r="31" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="47"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="45"/>
+    </row>
+    <row r="32" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="47"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="45"/>
+    </row>
+    <row r="33" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="47"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="45"/>
+    </row>
+    <row r="34" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="47"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="45"/>
+    </row>
+    <row r="35" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="47"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="45"/>
+    </row>
+    <row r="36" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="47"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="45"/>
+    </row>
+    <row r="37" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="47"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="45"/>
+    </row>
+    <row r="38" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="47"/>
+      <c r="B38" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="22" t="s">
+    <row r="39" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="22"/>
-      <c r="B40" s="23" t="s">
+    <row r="40" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="53"/>
+      <c r="B40" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="22"/>
-      <c r="B41" s="23" t="s">
+    <row r="41" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="53"/>
+      <c r="B41" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="31" t="s">
+    <row r="42" spans="1:3" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="33"/>
-      <c r="B43" s="30" t="s">
+    <row r="43" spans="1:3" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="55"/>
+      <c r="B43" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="32"/>
-      <c r="B44" s="28" t="s">
+    <row r="44" spans="1:3" s="11" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="56"/>
+      <c r="B44" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="31" t="s">
+    <row r="45" spans="1:3" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="32"/>
-      <c r="B46" s="26" t="s">
+    <row r="46" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="41"/>
+      <c r="B46" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="31" t="s">
+    <row r="47" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="32"/>
-      <c r="B48" s="26" t="s">
+    <row r="48" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="58"/>
+      <c r="B48" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="31" t="s">
+    <row r="49" spans="1:3" s="29" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="33"/>
-      <c r="B50" s="26" t="s">
+    <row r="50" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="51"/>
+      <c r="B50" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="32"/>
-      <c r="B51" s="26" t="s">
+    <row r="51" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="52"/>
+      <c r="B51" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="29" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1371,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446C6DD3-D0DA-421A-A1C2-0B773979D151}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1387,12 +1698,1413 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="31"/>
+    </row>
+    <row r="9" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3012661A-54FD-4F1D-9BDB-80048E13CF7C}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.08984375" customWidth="1"/>
+    <col min="2" max="2" width="125.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+      <c r="A12" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A15" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+      <c r="A16" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{ACAE6C84-601D-4EEB-AB86-8F95792919E9}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{424CEA3D-BEA6-4B9E-94A5-AA31028310E3}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E92BDDAD-FF4F-479E-96E0-24EB0AC6B895}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{3DEB9035-F458-46F6-8B11-25943522BCE3}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{DF78063B-F3A1-40FE-9F19-BED0781A6C37}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{508FC23D-CE49-430C-A4B7-61D86C1AC909}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{DAFD2348-6303-40E5-BE53-C03815DCC16B}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{CE942581-AF06-42A5-A534-04AB8342F734}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{0EB98B4F-EDDF-4E7F-A9EE-9562CCE27812}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{9F4EF2DF-A44F-4B64-83E3-18DFBA34881E}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{2691B685-0B92-47CF-93D9-38283BD5D721}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{E94B5B8E-3927-4656-A283-CB556069EB26}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{31441496-F5AB-46CC-B518-E63B0F220560}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{9808BA15-371C-4684-98E1-24108A211A63}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{540D1C7F-7A43-4DFE-B1D4-7E2B9D26DE22}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{76E56FBD-C265-4F4F-ADA3-E7E37D2331BC}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{BE038FE7-D3C4-4B7C-A73E-AD13E7F77BB1}"/>
+    <hyperlink ref="A18" r:id="rId18" xr:uid="{80EED44D-8E27-49D7-8978-01D31EA78CE8}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{F17FA7D7-B106-44D1-BDE5-BA17F567804C}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{7F687B31-7AD7-4A49-A6FD-DBE9B03424AE}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{E744C62C-CFF2-413C-A8A7-47707175C128}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30236705-075D-4641-A400-A3A5176BB269}">
+  <dimension ref="A1:C182"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.08984375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="60">
+        <v>44562</v>
+      </c>
+      <c r="C2" s="61"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60">
+        <v>44563</v>
+      </c>
+      <c r="C3" s="61"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60">
+        <v>44564</v>
+      </c>
+      <c r="C4" s="61"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="59"/>
+      <c r="B5" s="60">
+        <v>44565</v>
+      </c>
+      <c r="C5" s="61"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="59"/>
+      <c r="B6" s="60">
+        <v>44566</v>
+      </c>
+      <c r="C6" s="61"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="59"/>
+      <c r="B7" s="60">
+        <v>44567</v>
+      </c>
+      <c r="C7" s="61"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="59"/>
+      <c r="B8" s="60">
+        <v>44568</v>
+      </c>
+      <c r="C8" s="61"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="59"/>
+      <c r="B9" s="60">
+        <v>44569</v>
+      </c>
+      <c r="C9" s="63"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="59"/>
+      <c r="B10" s="60">
+        <v>44570</v>
+      </c>
+      <c r="C10" s="63"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="59"/>
+      <c r="B11" s="60">
+        <v>44571</v>
+      </c>
+      <c r="C11" s="63"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="59"/>
+      <c r="B12" s="60">
+        <v>44572</v>
+      </c>
+      <c r="C12" s="63"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="59"/>
+      <c r="B13" s="60">
+        <v>44573</v>
+      </c>
+      <c r="C13" s="63"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="59"/>
+      <c r="B14" s="60">
+        <v>44574</v>
+      </c>
+      <c r="C14" s="63"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="59"/>
+      <c r="B15" s="60">
+        <v>44575</v>
+      </c>
+      <c r="C15" s="63"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="59"/>
+      <c r="B16" s="60">
+        <v>44576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="59"/>
+      <c r="B17" s="60">
+        <v>44577</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="59"/>
+      <c r="B18" s="60">
+        <v>44578</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="59"/>
+      <c r="B19" s="60">
+        <v>44579</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="59"/>
+      <c r="B20" s="60">
+        <v>44580</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="59"/>
+      <c r="B21" s="60">
+        <v>44581</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="59"/>
+      <c r="B22" s="60">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="59"/>
+      <c r="B23" s="60">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="59"/>
+      <c r="B24" s="60">
+        <v>44584</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="59"/>
+      <c r="B25" s="60">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="59"/>
+      <c r="B26" s="60">
+        <v>44586</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="59"/>
+      <c r="B27" s="60">
+        <v>44587</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="59"/>
+      <c r="B28" s="60">
+        <v>44588</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="59"/>
+      <c r="B29" s="60">
+        <v>44589</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="59"/>
+      <c r="B30" s="60">
+        <v>44590</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="59"/>
+      <c r="B31" s="60">
+        <v>44591</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="59"/>
+      <c r="B32" s="60">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="60">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="62"/>
+      <c r="B34" s="60">
+        <v>44594</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="62"/>
+      <c r="B35" s="60">
+        <v>44595</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="62"/>
+      <c r="B36" s="60">
+        <v>44596</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="62"/>
+      <c r="B37" s="60">
+        <v>44597</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="62"/>
+      <c r="B38" s="60">
+        <v>44598</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="62"/>
+      <c r="B39" s="60">
+        <v>44599</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="62"/>
+      <c r="B40" s="60">
+        <v>44600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="62"/>
+      <c r="B41" s="60">
+        <v>44601</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="62"/>
+      <c r="B42" s="60">
+        <v>44602</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="62"/>
+      <c r="B43" s="60">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="62"/>
+      <c r="B44" s="60">
+        <v>44604</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="62"/>
+      <c r="B45" s="60">
+        <v>44605</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="62"/>
+      <c r="B46" s="60">
+        <v>44606</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="62"/>
+      <c r="B47" s="60">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="62"/>
+      <c r="B48" s="60">
+        <v>44608</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="62"/>
+      <c r="B49" s="60">
+        <v>44609</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="62"/>
+      <c r="B50" s="60">
+        <v>44610</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="62"/>
+      <c r="B51" s="60">
+        <v>44611</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="62"/>
+      <c r="B52" s="60">
+        <v>44612</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="62"/>
+      <c r="B53" s="60">
+        <v>44613</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="62"/>
+      <c r="B54" s="60">
+        <v>44614</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="62"/>
+      <c r="B55" s="60">
+        <v>44615</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="62"/>
+      <c r="B56" s="60">
+        <v>44616</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="62"/>
+      <c r="B57" s="60">
+        <v>44617</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="62"/>
+      <c r="B58" s="60">
+        <v>44618</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="62"/>
+      <c r="B59" s="60">
+        <v>44619</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="62"/>
+      <c r="B60" s="60">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="60">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="62"/>
+      <c r="B62" s="60">
+        <v>44622</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="62"/>
+      <c r="B63" s="60">
+        <v>44623</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="62"/>
+      <c r="B64" s="60">
+        <v>44624</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="62"/>
+      <c r="B65" s="60">
+        <v>44625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="62"/>
+      <c r="B66" s="60">
+        <v>44626</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="62"/>
+      <c r="B67" s="60">
+        <v>44627</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="62"/>
+      <c r="B68" s="60">
+        <v>44628</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="62"/>
+      <c r="B69" s="60">
+        <v>44629</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="62"/>
+      <c r="B70" s="60">
+        <v>44630</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="62"/>
+      <c r="B71" s="60">
+        <v>44631</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="62"/>
+      <c r="B72" s="60">
+        <v>44632</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="62"/>
+      <c r="B73" s="60">
+        <v>44633</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="62"/>
+      <c r="B74" s="60">
+        <v>44634</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" s="62"/>
+      <c r="B75" s="60">
+        <v>44635</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" s="62"/>
+      <c r="B76" s="60">
+        <v>44636</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="62"/>
+      <c r="B77" s="60">
+        <v>44637</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="62"/>
+      <c r="B78" s="60">
+        <v>44638</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="62"/>
+      <c r="B79" s="60">
+        <v>44639</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="62"/>
+      <c r="B80" s="60">
+        <v>44640</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="62"/>
+      <c r="B81" s="60">
+        <v>44641</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="62"/>
+      <c r="B82" s="60">
+        <v>44642</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="62"/>
+      <c r="B83" s="60">
+        <v>44643</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="62"/>
+      <c r="B84" s="60">
+        <v>44644</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="62"/>
+      <c r="B85" s="60">
+        <v>44645</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="62"/>
+      <c r="B86" s="60">
+        <v>44646</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="62"/>
+      <c r="B87" s="60">
+        <v>44647</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="62"/>
+      <c r="B88" s="60">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="62"/>
+      <c r="B89" s="60">
+        <v>44649</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="62"/>
+      <c r="B90" s="60">
+        <v>44650</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="62"/>
+      <c r="B91" s="60">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="B92" s="60">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="62"/>
+      <c r="B93" s="60">
+        <v>44653</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="62"/>
+      <c r="B94" s="60">
+        <v>44654</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="62"/>
+      <c r="B95" s="60">
+        <v>44655</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="62"/>
+      <c r="B96" s="60">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="62"/>
+      <c r="B97" s="60">
+        <v>44657</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="62"/>
+      <c r="B98" s="60">
+        <v>44658</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="62"/>
+      <c r="B99" s="60">
+        <v>44659</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="62"/>
+      <c r="B100" s="60">
+        <v>44660</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="62"/>
+      <c r="B101" s="60">
+        <v>44661</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="62"/>
+      <c r="B102" s="60">
+        <v>44662</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="62"/>
+      <c r="B103" s="60">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="62"/>
+      <c r="B104" s="60">
+        <v>44664</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="62"/>
+      <c r="B105" s="60">
+        <v>44665</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="62"/>
+      <c r="B106" s="60">
+        <v>44666</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="62"/>
+      <c r="B107" s="60">
+        <v>44667</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="62"/>
+      <c r="B108" s="60">
+        <v>44668</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="62"/>
+      <c r="B109" s="60">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="62"/>
+      <c r="B110" s="60">
+        <v>44670</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="62"/>
+      <c r="B111" s="60">
+        <v>44671</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="62"/>
+      <c r="B112" s="60">
+        <v>44672</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="62"/>
+      <c r="B113" s="60">
+        <v>44673</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="62"/>
+      <c r="B114" s="60">
+        <v>44674</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="62"/>
+      <c r="B115" s="60">
+        <v>44675</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="62"/>
+      <c r="B116" s="60">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="62"/>
+      <c r="B117" s="60">
+        <v>44677</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="62"/>
+      <c r="B118" s="60">
+        <v>44678</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="62"/>
+      <c r="B119" s="60">
+        <v>44679</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="62"/>
+      <c r="B120" s="60">
+        <v>44680</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="62"/>
+      <c r="B121" s="60">
+        <v>44681</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B122" s="60">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" s="62"/>
+      <c r="B123" s="60">
+        <v>44683</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" s="62"/>
+      <c r="B124" s="60">
+        <v>44684</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="62"/>
+      <c r="B125" s="60">
+        <v>44685</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="62"/>
+      <c r="B126" s="60">
+        <v>44686</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="62"/>
+      <c r="B127" s="60">
+        <v>44687</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="62"/>
+      <c r="B128" s="60">
+        <v>44688</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" s="62"/>
+      <c r="B129" s="60">
+        <v>44689</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" s="62"/>
+      <c r="B130" s="60">
+        <v>44690</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" s="62"/>
+      <c r="B131" s="60">
+        <v>44691</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" s="62"/>
+      <c r="B132" s="60">
+        <v>44692</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" s="62"/>
+      <c r="B133" s="60">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" s="62"/>
+      <c r="B134" s="60">
+        <v>44694</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" s="62"/>
+      <c r="B135" s="60">
+        <v>44695</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" s="62"/>
+      <c r="B136" s="60">
+        <v>44696</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" s="62"/>
+      <c r="B137" s="60">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" s="62"/>
+      <c r="B138" s="60">
+        <v>44698</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" s="62"/>
+      <c r="B139" s="60">
+        <v>44699</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" s="62"/>
+      <c r="B140" s="60">
+        <v>44700</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="62"/>
+      <c r="B141" s="60">
+        <v>44701</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" s="62"/>
+      <c r="B142" s="60">
+        <v>44702</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" s="62"/>
+      <c r="B143" s="60">
+        <v>44703</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" s="62"/>
+      <c r="B144" s="60">
+        <v>44704</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" s="62"/>
+      <c r="B145" s="60">
+        <v>44705</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" s="62"/>
+      <c r="B146" s="60">
+        <v>44706</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" s="62"/>
+      <c r="B147" s="60">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" s="62"/>
+      <c r="B148" s="60">
+        <v>44708</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" s="62"/>
+      <c r="B149" s="60">
+        <v>44709</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" s="62"/>
+      <c r="B150" s="60">
+        <v>44710</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" s="62"/>
+      <c r="B151" s="60">
+        <v>44711</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" s="62"/>
+      <c r="B152" s="60">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B153" s="60">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="62"/>
+      <c r="B154" s="60">
+        <v>44714</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="62"/>
+      <c r="B155" s="60">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="62"/>
+      <c r="B156" s="60">
+        <v>44716</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" s="62"/>
+      <c r="B157" s="60">
+        <v>44717</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" s="62"/>
+      <c r="B158" s="60">
+        <v>44718</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" s="62"/>
+      <c r="B159" s="60">
+        <v>44719</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" s="62"/>
+      <c r="B160" s="60">
+        <v>44720</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" s="62"/>
+      <c r="B161" s="60">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" s="62"/>
+      <c r="B162" s="60">
+        <v>44722</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" s="62"/>
+      <c r="B163" s="60">
+        <v>44723</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" s="62"/>
+      <c r="B164" s="60">
+        <v>44724</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" s="62"/>
+      <c r="B165" s="60">
+        <v>44725</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166" s="62"/>
+      <c r="B166" s="60">
+        <v>44726</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A167" s="62"/>
+      <c r="B167" s="60">
+        <v>44727</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A168" s="62"/>
+      <c r="B168" s="60">
+        <v>44728</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" s="62"/>
+      <c r="B169" s="60">
+        <v>44729</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" s="62"/>
+      <c r="B170" s="60">
+        <v>44730</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" s="62"/>
+      <c r="B171" s="60">
+        <v>44731</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" s="62"/>
+      <c r="B172" s="60">
+        <v>44732</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" s="62"/>
+      <c r="B173" s="60">
+        <v>44733</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" s="62"/>
+      <c r="B174" s="60">
+        <v>44734</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" s="62"/>
+      <c r="B175" s="60">
+        <v>44735</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176" s="62"/>
+      <c r="B176" s="60">
+        <v>44736</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177" s="62"/>
+      <c r="B177" s="60">
+        <v>44737</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178" s="62"/>
+      <c r="B178" s="60">
+        <v>44738</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" s="62"/>
+      <c r="B179" s="60">
+        <v>44739</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180" s="62"/>
+      <c r="B180" s="60">
+        <v>44740</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181" s="62"/>
+      <c r="B181" s="60">
+        <v>44741</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" s="62"/>
+      <c r="B182" s="60">
+        <v>44742</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A153:A182"/>
+    <mergeCell ref="A2:A32"/>
+    <mergeCell ref="A33:A60"/>
+    <mergeCell ref="A61:A91"/>
+    <mergeCell ref="A92:A121"/>
+    <mergeCell ref="A122:A152"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>